<commit_message>
finalize prac10: reports, remove unused files
</commit_message>
<xml_diff>
--- a/PL/prac10/informe/PCP2022UO283319PRAC10.xlsx
+++ b/PL/prac10/informe/PCP2022UO283319PRAC10.xlsx
@@ -1655,11 +1655,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="1179645605"/>
-        <c:axId val="237504827"/>
+        <c:axId val="144989157"/>
+        <c:axId val="1514619203"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1179645605"/>
+        <c:axId val="144989157"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1711,10 +1711,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237504827"/>
+        <c:crossAx val="1514619203"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="237504827"/>
+        <c:axId val="1514619203"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15.0"/>
@@ -1790,7 +1790,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1179645605"/>
+        <c:crossAx val="144989157"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2001,11 +2001,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="324183319"/>
-        <c:axId val="297319427"/>
+        <c:axId val="1233555537"/>
+        <c:axId val="136530362"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324183319"/>
+        <c:axId val="1233555537"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2057,10 +2057,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297319427"/>
+        <c:crossAx val="136530362"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297319427"/>
+        <c:axId val="136530362"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2135,7 +2135,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324183319"/>
+        <c:crossAx val="1233555537"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2381,11 +2381,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="1414722943"/>
-        <c:axId val="1880417758"/>
+        <c:axId val="1105921002"/>
+        <c:axId val="1636319787"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1414722943"/>
+        <c:axId val="1105921002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2437,10 +2437,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1880417758"/>
+        <c:crossAx val="1636319787"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1880417758"/>
+        <c:axId val="1636319787"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2515,7 +2515,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1414722943"/>
+        <c:crossAx val="1105921002"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2726,11 +2726,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1905347542"/>
-        <c:axId val="1225419068"/>
+        <c:axId val="1760676604"/>
+        <c:axId val="2005807538"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1905347542"/>
+        <c:axId val="1760676604"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2782,10 +2782,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1225419068"/>
+        <c:crossAx val="2005807538"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1225419068"/>
+        <c:axId val="2005807538"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2860,7 +2860,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1905347542"/>
+        <c:crossAx val="1760676604"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3078,11 +3078,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="25767058"/>
-        <c:axId val="1598421931"/>
+        <c:axId val="1591481597"/>
+        <c:axId val="339565191"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="25767058"/>
+        <c:axId val="1591481597"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3134,10 +3134,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1598421931"/>
+        <c:crossAx val="339565191"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1598421931"/>
+        <c:axId val="339565191"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3212,7 +3212,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25767058"/>
+        <c:crossAx val="1591481597"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3373,11 +3373,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="1654090108"/>
-        <c:axId val="692816990"/>
+        <c:axId val="1435008924"/>
+        <c:axId val="1711389415"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1654090108"/>
+        <c:axId val="1435008924"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3429,10 +3429,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="692816990"/>
+        <c:crossAx val="1711389415"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="692816990"/>
+        <c:axId val="1711389415"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3507,7 +3507,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1654090108"/>
+        <c:crossAx val="1435008924"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3723,11 +3723,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="326869281"/>
-        <c:axId val="25491375"/>
+        <c:axId val="1484549255"/>
+        <c:axId val="873491071"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="326869281"/>
+        <c:axId val="1484549255"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3779,10 +3779,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25491375"/>
+        <c:crossAx val="873491071"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="25491375"/>
+        <c:axId val="873491071"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3857,7 +3857,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326869281"/>
+        <c:crossAx val="1484549255"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4104,11 +4104,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="1661131329"/>
-        <c:axId val="1601784096"/>
+        <c:axId val="1425332967"/>
+        <c:axId val="584290665"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1661131329"/>
+        <c:axId val="1425332967"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4160,10 +4160,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1601784096"/>
+        <c:crossAx val="584290665"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1601784096"/>
+        <c:axId val="584290665"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4238,7 +4238,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1661131329"/>
+        <c:crossAx val="1425332967"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4423,11 +4423,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="719054533"/>
-        <c:axId val="1299004617"/>
+        <c:axId val="290274036"/>
+        <c:axId val="1449517735"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="719054533"/>
+        <c:axId val="290274036"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="6000.0"/>
@@ -4480,10 +4480,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1299004617"/>
+        <c:crossAx val="1449517735"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1299004617"/>
+        <c:axId val="1449517735"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.02"/>
@@ -4559,7 +4559,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="719054533"/>
+        <c:crossAx val="290274036"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4715,11 +4715,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="340366336"/>
-        <c:axId val="734427871"/>
+        <c:axId val="1601366568"/>
+        <c:axId val="844493489"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="340366336"/>
+        <c:axId val="1601366568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4771,10 +4771,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="734427871"/>
+        <c:crossAx val="844493489"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="734427871"/>
+        <c:axId val="844493489"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4849,7 +4849,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340366336"/>
+        <c:crossAx val="1601366568"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5030,11 +5030,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="172942892"/>
-        <c:axId val="372941239"/>
+        <c:axId val="1246535613"/>
+        <c:axId val="1768163044"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="172942892"/>
+        <c:axId val="1246535613"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5086,10 +5086,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="372941239"/>
+        <c:crossAx val="1768163044"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="372941239"/>
+        <c:axId val="1768163044"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5164,7 +5164,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172942892"/>
+        <c:crossAx val="1246535613"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5325,11 +5325,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="1702667538"/>
-        <c:axId val="245264530"/>
+        <c:axId val="941143182"/>
+        <c:axId val="1837178776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1702667538"/>
+        <c:axId val="941143182"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5381,10 +5381,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245264530"/>
+        <c:crossAx val="1837178776"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245264530"/>
+        <c:axId val="1837178776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5459,7 +5459,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1702667538"/>
+        <c:crossAx val="941143182"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5610,11 +5610,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1833410859"/>
-        <c:axId val="836644936"/>
+        <c:axId val="935984250"/>
+        <c:axId val="1765087884"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1833410859"/>
+        <c:axId val="935984250"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5666,10 +5666,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="836644936"/>
+        <c:crossAx val="1765087884"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="836644936"/>
+        <c:axId val="1765087884"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5744,7 +5744,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1833410859"/>
+        <c:crossAx val="935984250"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5931,11 +5931,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="1790085980"/>
-        <c:axId val="625897907"/>
+        <c:axId val="727442640"/>
+        <c:axId val="2041840432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1790085980"/>
+        <c:axId val="727442640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5987,10 +5987,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="625897907"/>
+        <c:crossAx val="2041840432"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="625897907"/>
+        <c:axId val="2041840432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6065,7 +6065,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1790085980"/>
+        <c:crossAx val="727442640"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>